<commit_message>
ZSS-452 Inserting a row at non-selected sheet with API doesn't work
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/452-insertAtAnotherSheet.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/452-insertAtAnotherSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="18195" windowHeight="7230"/>
@@ -10,28 +10,75 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>select this sheet</t>
   </si>
   <si>
     <t>one row inserted above this row</t>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -86,75 +133,301 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="55777920"/>
+        <c:axId val="72388992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="55777920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72388992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="72388992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55777920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Sunset.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2581275" y="2247900"/>
+          <a:ext cx="2286000" cy="1714500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -165,7 +438,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -445,129 +718,131 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B1" s="2">
         <v>1</v>
       </c>
       <c r="C1" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>3</v>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
       <c r="C3" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>4</v>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>6</v>
+      <c r="A6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
       </c>
       <c r="C6" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>7</v>
+      <c r="A7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>7</v>
       </c>
       <c r="C7" s="3">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>8</v>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>8</v>
       </c>
       <c r="C8" s="3">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>9</v>
+      <c r="A9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>9</v>
       </c>
       <c r="C9" s="3">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>10</v>
+      <c r="A10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -579,7 +854,7 @@
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -590,6 +865,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>